<commit_message>
Update video start time and word occurrence in Task.svelte and mathStimuli.ts
</commit_message>
<xml_diff>
--- a/transformations/mathStimuli.xlsx
+++ b/transformations/mathStimuli.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\248049\Desktop\MSCA_23 SEp\Experiment Project\Maths Task Stimuli_Task 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelavojtechovska/Desktop/Svelte/fss-mu-multitask-experiment/transformations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE429122-CD45-4965-B5EF-D29536C7C16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FA737C-9D5E-134A-945B-9105E2F87004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0EBB0231-4E46-4B4E-A759-A65CFD5AA6A5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{0EBB0231-4E46-4B4E-A759-A65CFD5AA6A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -994,16 +994,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6066E54B-0025-48FF-B7D4-A54F7F6D5F59}">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F202" sqref="F202"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1823,7 +1823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2043,7 +2043,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2843,7 +2843,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3043,7 +3043,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3323,7 +3323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>19</v>
       </c>
       <c r="D119">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E119">
         <v>37</v>
@@ -3383,7 +3383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4023,7 +4023,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4143,7 +4143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -4363,7 +4363,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -4463,7 +4463,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -4523,7 +4523,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
@@ -4863,7 +4863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>194</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
@@ -4943,7 +4943,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>197</v>
       </c>
@@ -4963,7 +4963,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>198</v>
       </c>
@@ -4983,7 +4983,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>199</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>200</v>
       </c>
@@ -5036,9 +5036,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>8</v>
       </c>
@@ -5052,7 +5052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>48</v>
       </c>
@@ -5066,7 +5066,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>22</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>200</v>
       </c>
@@ -5094,7 +5094,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>24</v>
       </c>
@@ -5108,7 +5108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>58</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>45</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>58</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>69</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>27</v>
       </c>
@@ -5178,7 +5178,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>102</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>60</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>15</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>17</v>
       </c>
@@ -5234,7 +5234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>17</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>11</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>21</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>22</v>
       </c>
@@ -5304,7 +5304,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>41</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>31</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>65</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>25</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>15</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>27</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>37</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>65</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>18</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>44</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>21</v>
       </c>
@@ -5458,7 +5458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
@@ -5472,7 +5472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>18</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>8</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>19</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>14</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>34</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>46</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>54</v>
       </c>
@@ -5584,7 +5584,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>45</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>10</v>
       </c>
@@ -5612,7 +5612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>16</v>
       </c>
@@ -5626,7 +5626,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>19</v>
       </c>
@@ -5640,7 +5640,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>23</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>31</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>22</v>
       </c>
@@ -5682,7 +5682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>23</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>47</v>
       </c>
@@ -5738,7 +5738,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>21</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>26</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>45</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>31</v>
       </c>
@@ -5794,7 +5794,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>12</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>15</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>18</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>13</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>64</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>74</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>13</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>56</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>48</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>57</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>23</v>
       </c>
@@ -5948,7 +5948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>20</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>48</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>12</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>63</v>
       </c>
@@ -6004,7 +6004,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>56</v>
       </c>
@@ -6018,7 +6018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>45</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>30</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>65</v>
       </c>
@@ -6060,7 +6060,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>15</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>30</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>20</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>35</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>56</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>45</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>57</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>56</v>
       </c>
@@ -6172,7 +6172,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>59</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>30</v>
       </c>
@@ -6200,7 +6200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>5</v>
       </c>
@@ -6214,7 +6214,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>89</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>4</v>
       </c>
@@ -6242,7 +6242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>62</v>
       </c>
@@ -6256,7 +6256,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>30</v>
       </c>
@@ -6270,7 +6270,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>78</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>56</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
@@ -6312,7 +6312,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>45</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>23</v>
       </c>
@@ -6340,7 +6340,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>45</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>12</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>56</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>23</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>45</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Update math stimuli content and responses in mathStimuli.ts; modify execution count and Python version in prepareFromExcel.ipynb
</commit_message>
<xml_diff>
--- a/transformations/mathStimuli.xlsx
+++ b/transformations/mathStimuli.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelavojtechovska/Desktop/Svelte/fss-mu-multitask-experiment/transformations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\248049\Desktop\Misa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FA737C-9D5E-134A-945B-9105E2F87004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B7E12B9-BDC3-4EB9-8816-7A5EC2DE3617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{0EBB0231-4E46-4B4E-A759-A65CFD5AA6A5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0EBB0231-4E46-4B4E-A759-A65CFD5AA6A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -580,9 +580,6 @@
     <t>(6 ÷ 2) + 3 = ?</t>
   </si>
   <si>
-    <t>12 - ( 4 + 2) = ?</t>
-  </si>
-  <si>
     <t>(15 - 3) ÷ 3 = ?</t>
   </si>
   <si>
@@ -626,6 +623,9 @@
   </si>
   <si>
     <t>7 + (10 - 2) ÷ 2 = ?</t>
+  </si>
+  <si>
+    <t>15 - ( 1 + 3) = ?</t>
   </si>
 </sst>
 </file>
@@ -661,8 +661,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,9 +697,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -736,7 +737,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -842,7 +843,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -984,7 +985,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -994,16 +995,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6066E54B-0025-48FF-B7D4-A54F7F6D5F59}">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I182" sqref="I182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1083,7 +1084,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1143,7 +1144,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1203,7 +1204,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1223,7 +1224,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1243,7 +1244,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1263,7 +1264,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1283,7 +1284,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1303,7 +1304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1363,7 +1364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1383,7 +1384,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1403,7 +1404,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1423,7 +1424,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1443,7 +1444,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1463,7 +1464,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1543,7 +1544,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1603,7 +1604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1623,7 +1624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1643,7 +1644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1663,7 +1664,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1683,7 +1684,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1723,7 +1724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1763,7 +1764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1823,7 +1824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1843,7 +1844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1863,7 +1864,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1903,7 +1904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1923,7 +1924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1943,7 +1944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1963,7 +1964,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1983,7 +1984,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2023,7 +2024,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2043,7 +2044,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2103,7 +2104,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2123,7 +2124,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2163,7 +2164,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2183,7 +2184,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2203,7 +2204,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2243,7 +2244,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2303,7 +2304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2343,7 +2344,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2363,7 +2364,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2383,7 +2384,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2403,7 +2404,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2423,7 +2424,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2463,7 +2464,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2483,7 +2484,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2523,7 +2524,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2543,7 +2544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2563,7 +2564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2583,7 +2584,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2603,7 +2604,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2623,7 +2624,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2643,7 +2644,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2663,7 +2664,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2683,7 +2684,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2703,7 +2704,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2723,7 +2724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2763,7 +2764,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2783,7 +2784,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2803,7 +2804,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2823,7 +2824,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2843,7 +2844,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2863,7 +2864,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2883,7 +2884,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2903,7 +2904,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2923,7 +2924,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2943,7 +2944,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2963,7 +2964,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2983,7 +2984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3023,7 +3024,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3043,7 +3044,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3063,7 +3064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3103,7 +3104,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3123,7 +3124,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3163,7 +3164,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3203,7 +3204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3223,7 +3224,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3243,7 +3244,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3263,7 +3264,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -3283,7 +3284,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -3303,7 +3304,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -3323,7 +3324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -3343,7 +3344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -3363,7 +3364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -3383,7 +3384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3403,7 +3404,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3423,7 +3424,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3443,18 +3444,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C123">
         <v>48</v>
       </c>
       <c r="D123">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E123">
         <v>65</v>
@@ -3463,7 +3464,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3483,7 +3484,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3503,7 +3504,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3523,7 +3524,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3543,7 +3544,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3563,7 +3564,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3583,7 +3584,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3603,7 +3604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3623,7 +3624,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3643,7 +3644,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3663,7 +3664,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3683,7 +3684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3703,7 +3704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3723,7 +3724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3743,7 +3744,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3763,7 +3764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3783,7 +3784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3803,7 +3804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -3823,7 +3824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -3843,7 +3844,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -3863,7 +3864,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3883,7 +3884,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3903,7 +3904,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3923,7 +3924,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -3943,7 +3944,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -3963,7 +3964,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -3983,7 +3984,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -4003,7 +4004,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -4023,7 +4024,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -4063,7 +4064,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -4083,7 +4084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -4103,7 +4104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -4123,7 +4124,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -4143,7 +4144,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -4163,7 +4164,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -4183,7 +4184,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -4203,7 +4204,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -4223,7 +4224,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -4243,7 +4244,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -4263,7 +4264,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -4283,7 +4284,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -4303,7 +4304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -4323,7 +4324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -4343,7 +4344,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -4363,7 +4364,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -4383,7 +4384,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -4403,7 +4404,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -4423,7 +4424,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -4443,7 +4444,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -4463,7 +4464,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -4483,7 +4484,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -4503,7 +4504,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -4523,7 +4524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -4543,7 +4544,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -4563,7 +4564,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -4583,7 +4584,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -4603,7 +4604,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -4623,7 +4624,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -4643,7 +4644,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -4663,7 +4664,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -4683,18 +4684,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
-      <c r="B185" t="s">
-        <v>181</v>
+      <c r="B185" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="C185">
         <v>9</v>
       </c>
       <c r="D185">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E185">
         <v>35</v>
@@ -4703,7 +4704,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -4723,12 +4724,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C187">
         <v>31</v>
@@ -4743,12 +4744,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C188">
         <v>5</v>
@@ -4763,12 +4764,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C189">
         <v>26</v>
@@ -4783,12 +4784,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C190">
         <v>2</v>
@@ -4803,12 +4804,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C191">
         <v>4</v>
@@ -4823,12 +4824,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C192">
         <v>19</v>
@@ -4843,12 +4844,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C193">
         <v>4</v>
@@ -4863,12 +4864,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C194">
         <v>15</v>
@@ -4883,12 +4884,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C195">
         <v>23</v>
@@ -4903,12 +4904,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C196">
         <v>20</v>
@@ -4923,12 +4924,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C197">
         <v>10</v>
@@ -4943,12 +4944,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C198">
         <v>11</v>
@@ -4963,12 +4964,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C199">
         <v>12</v>
@@ -4983,12 +4984,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C200">
         <v>15</v>
@@ -5003,18 +5004,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C201">
         <v>9</v>
       </c>
       <c r="D201">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E201">
         <v>21</v>
@@ -5036,9 +5037,9 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>8</v>
       </c>
@@ -5052,7 +5053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>48</v>
       </c>
@@ -5066,7 +5067,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>22</v>
       </c>
@@ -5080,7 +5081,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>200</v>
       </c>
@@ -5094,7 +5095,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>24</v>
       </c>
@@ -5108,7 +5109,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>58</v>
       </c>
@@ -5122,7 +5123,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>45</v>
       </c>
@@ -5136,7 +5137,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>58</v>
       </c>
@@ -5150,7 +5151,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>69</v>
       </c>
@@ -5164,7 +5165,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>27</v>
       </c>
@@ -5178,7 +5179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>102</v>
       </c>
@@ -5192,7 +5193,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>60</v>
       </c>
@@ -5206,7 +5207,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
@@ -5220,7 +5221,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>17</v>
       </c>
@@ -5234,7 +5235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -5248,7 +5249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>17</v>
       </c>
@@ -5262,7 +5263,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -5276,7 +5277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>21</v>
       </c>
@@ -5290,7 +5291,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>22</v>
       </c>
@@ -5304,7 +5305,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>41</v>
       </c>
@@ -5318,7 +5319,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31</v>
       </c>
@@ -5332,7 +5333,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>65</v>
       </c>
@@ -5346,7 +5347,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>25</v>
       </c>
@@ -5360,7 +5361,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -5374,7 +5375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>27</v>
       </c>
@@ -5388,7 +5389,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>37</v>
       </c>
@@ -5402,7 +5403,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>65</v>
       </c>
@@ -5416,7 +5417,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>18</v>
       </c>
@@ -5430,7 +5431,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>44</v>
       </c>
@@ -5444,7 +5445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>21</v>
       </c>
@@ -5458,7 +5459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>20</v>
       </c>
@@ -5472,7 +5473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>18</v>
       </c>
@@ -5486,7 +5487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>20</v>
       </c>
@@ -5500,7 +5501,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>8</v>
       </c>
@@ -5514,7 +5515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>19</v>
       </c>
@@ -5528,7 +5529,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>14</v>
       </c>
@@ -5542,7 +5543,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -5556,7 +5557,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>46</v>
       </c>
@@ -5570,7 +5571,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>54</v>
       </c>
@@ -5584,7 +5585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>45</v>
       </c>
@@ -5598,7 +5599,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10</v>
       </c>
@@ -5612,7 +5613,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>16</v>
       </c>
@@ -5626,7 +5627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>19</v>
       </c>
@@ -5640,7 +5641,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>23</v>
       </c>
@@ -5654,7 +5655,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>31</v>
       </c>
@@ -5668,7 +5669,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>22</v>
       </c>
@@ -5682,7 +5683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -5696,7 +5697,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -5710,7 +5711,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>23</v>
       </c>
@@ -5724,7 +5725,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -5738,7 +5739,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>21</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>26</v>
       </c>
@@ -5766,7 +5767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>45</v>
       </c>
@@ -5780,7 +5781,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>31</v>
       </c>
@@ -5794,7 +5795,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>12</v>
       </c>
@@ -5808,7 +5809,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>15</v>
       </c>
@@ -5822,7 +5823,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>18</v>
       </c>
@@ -5836,7 +5837,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>13</v>
       </c>
@@ -5850,7 +5851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>64</v>
       </c>
@@ -5864,7 +5865,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>74</v>
       </c>
@@ -5878,7 +5879,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>13</v>
       </c>
@@ -5892,7 +5893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>56</v>
       </c>
@@ -5906,7 +5907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>48</v>
       </c>
@@ -5920,7 +5921,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>57</v>
       </c>
@@ -5934,7 +5935,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>23</v>
       </c>
@@ -5948,7 +5949,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>20</v>
       </c>
@@ -5962,7 +5963,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>48</v>
       </c>
@@ -5976,7 +5977,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>12</v>
       </c>
@@ -5990,7 +5991,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>63</v>
       </c>
@@ -6004,7 +6005,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>56</v>
       </c>
@@ -6018,7 +6019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>45</v>
       </c>
@@ -6032,7 +6033,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>30</v>
       </c>
@@ -6046,7 +6047,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>65</v>
       </c>
@@ -6060,7 +6061,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>15</v>
       </c>
@@ -6074,7 +6075,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>30</v>
       </c>
@@ -6088,7 +6089,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>20</v>
       </c>
@@ -6102,7 +6103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>35</v>
       </c>
@@ -6116,7 +6117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>56</v>
       </c>
@@ -6130,7 +6131,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>45</v>
       </c>
@@ -6144,7 +6145,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>57</v>
       </c>
@@ -6158,7 +6159,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>56</v>
       </c>
@@ -6172,7 +6173,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>59</v>
       </c>
@@ -6186,7 +6187,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>30</v>
       </c>
@@ -6200,7 +6201,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>5</v>
       </c>
@@ -6214,7 +6215,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>89</v>
       </c>
@@ -6228,7 +6229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>4</v>
       </c>
@@ -6242,7 +6243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>62</v>
       </c>
@@ -6256,7 +6257,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>30</v>
       </c>
@@ -6270,7 +6271,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>78</v>
       </c>
@@ -6284,7 +6285,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>56</v>
       </c>
@@ -6298,7 +6299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -6312,7 +6313,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>45</v>
       </c>
@@ -6326,7 +6327,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>23</v>
       </c>
@@ -6340,7 +6341,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>45</v>
       </c>
@@ -6354,7 +6355,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>12</v>
       </c>
@@ -6368,7 +6369,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>56</v>
       </c>
@@ -6382,7 +6383,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>23</v>
       </c>
@@ -6396,7 +6397,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>45</v>
       </c>
@@ -6410,7 +6411,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>78</v>
       </c>
@@ -6429,18 +6430,12 @@
     <cfRule type="expression" dxfId="1" priority="6">
       <formula>COUNTIF($A$1:$E$1, A1) &gt; 1</formula>
     </cfRule>
-    <cfRule type="expression" priority="4">
-      <formula>COUNTIF($A$1:$E$1, A1) &gt; 1</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:D1048576">
-    <cfRule type="expression" priority="5">
-      <formula>COUNTIF($A$1:$E$1, A1) &gt; 1</formula>
-    </cfRule>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
     <cfRule type="expression" priority="3">
       <formula>COUNTIF($A$1:$E$1, A1) &gt; 1</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
     <cfRule type="duplicateValues" priority="2"/>

</xml_diff>